<commit_message>
Updated remainder of Excel templates
</commit_message>
<xml_diff>
--- a/ExcelTemplates/FutureShopTemplate-Invalid-ExtraTag.xlsx
+++ b/ExcelTemplates/FutureShopTemplate-Invalid-ExtraTag.xlsx
@@ -1,14 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16380"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -100,18 +103,6 @@
     <t>Product_Tags</t>
   </si>
   <si>
-    <t>element_name</t>
-  </si>
-  <si>
-    <t>element_attribute_name</t>
-  </si>
-  <si>
-    <t>element_attribute_value</t>
-  </si>
-  <si>
-    <t>element_content_attribute_name</t>
-  </si>
-  <si>
     <t>div</t>
   </si>
   <si>
@@ -121,9 +112,6 @@
     <t>item-inner clearfix</t>
   </si>
   <si>
-    <t>Attribute_Name</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -140,6 +128,21 @@
   </si>
   <si>
     <t>prod-price</t>
+  </si>
+  <si>
+    <t>html_tag</t>
+  </si>
+  <si>
+    <t>html_tag_attribute_name</t>
+  </si>
+  <si>
+    <t>html_tag_attribute_value</t>
+  </si>
+  <si>
+    <t>content_location</t>
+  </si>
+  <si>
+    <t>Item_Attribute_Name</t>
   </si>
 </sst>
 </file>
@@ -194,8 +197,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -491,17 +522,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -509,7 +540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -517,7 +548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -525,180 +556,180 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>